<commit_message>
Updated plots after Excel from Ansys model changes
</commit_message>
<xml_diff>
--- a/3_ML/Part B - Matlab Model/wavenumber-frequency curve.xlsx
+++ b/3_ML/Part B - Matlab Model/wavenumber-frequency curve.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2BDA74-33EB-42DD-9DC4-BBFF900ED1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{6A15CA82-5337-48B6-BCBF-DA78EBE36219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFD56D1E-9AD7-417D-B317-41794BB7EF32}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -642,23 +642,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
@@ -781,157 +773,157 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$52</c:f>
+              <c:f>Sheet1!$C$4:$C$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
                 <c:pt idx="0">
+                  <c:v>1.963495375E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9269907499999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5.8904861249999996E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>7.8539814999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>9.8174768750000002E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.11780972249999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.13744467625000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0.15707963</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.17671458374999999</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.1963495375</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>0.21598449125000002</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.23561944499999998</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.25525439875</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.27488935250000002</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.29452430625000003</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>0.31415926</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>0.33379421375000001</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>0.35342916749999997</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>0.37306412125000005</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>0.39269907500000001</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>0.41233402875000003</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>0.43196898250000004</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>0.45160393625</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>0.47123888999999997</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>0.49087384374999998</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>0.5105087975</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>0.53014375125000002</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>0.54977870500000003</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>0.56941365874999994</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>0.58904861250000007</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>0.60868356625000009</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>0.62831851999999999</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>0.64795347375000001</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>0.66758842750000003</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>0.68722338125000004</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>0.70685833499999995</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>0.72649328874999997</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>0.74612824250000009</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>0.76576319625000011</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>0.78539815000000002</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>0.80503310375000003</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>0.82466805750000005</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>0.84430301125000007</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>0.86393796500000009</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>0.8835729187500001</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>0.90320787250000001</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>0.92284282625000003</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.94247777999999993</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.96211273374999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$6:$F$52</c:f>
+              <c:f>Sheet1!$F$4:$F$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="47"/>
@@ -2128,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2138,21 +2130,21 @@
     <col min="3" max="3" width="15.21875" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" style="8" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
     <col min="9" max="9" width="97.44140625" customWidth="1"/>
     <col min="18" max="18" width="9.109375" style="8"/>
     <col min="19" max="19" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="22"/>
       <c r="R1"/>
     </row>
     <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
@@ -2167,7 +2159,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
@@ -2196,7 +2188,7 @@
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="9" t="s">
         <v>71</v>
       </c>
       <c r="G3" s="9"/>
@@ -2230,14 +2222,17 @@
         <f>2*3.1415926/B4</f>
         <v>1.963495375E-2</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="21">
+        <f>S7</f>
+        <v>20.734940000000002</v>
+      </c>
       <c r="E4" s="10">
         <f>2*3.1415926*D4/C4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="26">
+        <v>6635.180800000001</v>
+      </c>
+      <c r="F4" s="23">
         <f>2*PI()*D4</f>
-        <v>0</v>
+        <v>130.28147035325031</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -2265,14 +2260,17 @@
         <f t="shared" ref="C5:C58" si="1">2*3.1415926/B5</f>
         <v>3.9269907499999999E-2</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="21">
+        <f t="shared" ref="D5:D58" si="2">S8</f>
+        <v>20.773472000000002</v>
+      </c>
       <c r="E5" s="10">
-        <f t="shared" ref="E5:E58" si="2">2*3.1415926*D5/C5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="26">
-        <f t="shared" ref="F5:F58" si="3">2*PI()*D5</f>
-        <v>0</v>
+        <f>2*3.1415926*D5/C5</f>
+        <v>3323.7555200000002</v>
+      </c>
+      <c r="F5" s="23">
+        <f>2*PI()*D5</f>
+        <v>130.52357404950655</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -2301,16 +2299,16 @@
         <v>5.8904861249999996E-2</v>
       </c>
       <c r="D6" s="21">
-        <f>S7</f>
-        <v>20.734940000000002</v>
+        <f t="shared" si="2"/>
+        <v>20.792885999999999</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" si="2"/>
-        <v>2211.7269333333338</v>
-      </c>
-      <c r="F6" s="26">
-        <f t="shared" si="3"/>
-        <v>130.28147035325031</v>
+        <f t="shared" ref="E6:E58" si="3">2*3.1415926*D6/C6</f>
+        <v>2217.9078399999999</v>
+      </c>
+      <c r="F6" s="23">
+        <f t="shared" ref="F6:F58" si="4">2*PI()*D6</f>
+        <v>130.64555580906011</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -2358,16 +2356,16 @@
         <v>7.8539814999999999E-2</v>
       </c>
       <c r="D7" s="21">
-        <f t="shared" ref="D7:D58" si="4">S8</f>
-        <v>20.773472000000002</v>
+        <f t="shared" si="2"/>
+        <v>20.829048</v>
       </c>
       <c r="E7" s="10">
-        <f t="shared" si="2"/>
-        <v>1661.8777600000001</v>
-      </c>
-      <c r="F7" s="26">
         <f t="shared" si="3"/>
-        <v>130.52357404950655</v>
+        <v>1666.3238400000002</v>
+      </c>
+      <c r="F7" s="23">
+        <f t="shared" si="4"/>
+        <v>130.87276835613835</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -2414,16 +2412,16 @@
         <v>9.8174768750000002E-2</v>
       </c>
       <c r="D8" s="21">
+        <f t="shared" si="2"/>
+        <v>21.050971000000001</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="3"/>
+        <v>1347.262144</v>
+      </c>
+      <c r="F8" s="23">
         <f t="shared" si="4"/>
-        <v>20.792885999999999</v>
-      </c>
-      <c r="E8" s="10">
-        <f t="shared" si="2"/>
-        <v>1330.744704</v>
-      </c>
-      <c r="F8" s="26">
-        <f t="shared" si="3"/>
-        <v>130.64555580906011</v>
+        <v>132.26715168906355</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -2468,16 +2466,16 @@
         <v>0.11780972249999999</v>
       </c>
       <c r="D9" s="21">
+        <f t="shared" si="2"/>
+        <v>21.619999</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="3"/>
+        <v>1153.0666133333334</v>
+      </c>
+      <c r="F9" s="23">
         <f t="shared" si="4"/>
-        <v>20.829048</v>
-      </c>
-      <c r="E9" s="10">
-        <f t="shared" si="2"/>
-        <v>1110.8825600000002</v>
-      </c>
-      <c r="F9" s="26">
-        <f t="shared" si="3"/>
-        <v>130.87276835613835</v>
+        <v>135.84246005803735</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -2520,16 +2518,16 @@
         <v>0.13744467625000001</v>
       </c>
       <c r="D10" s="21">
+        <f t="shared" si="2"/>
+        <v>22.582768000000002</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="3"/>
+        <v>1032.3551085714287</v>
+      </c>
+      <c r="F10" s="23">
         <f t="shared" si="4"/>
-        <v>21.050971000000001</v>
-      </c>
-      <c r="E10" s="10">
-        <f t="shared" si="2"/>
-        <v>962.33010285714283</v>
-      </c>
-      <c r="F10" s="26">
-        <f t="shared" si="3"/>
-        <v>132.26715168906355</v>
+        <v>141.89171609304535</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -2572,16 +2570,16 @@
         <v>0.15707963</v>
       </c>
       <c r="D11" s="21">
+        <f t="shared" si="2"/>
+        <v>23.925006</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="3"/>
+        <v>957.00023999999996</v>
+      </c>
+      <c r="F11" s="23">
         <f t="shared" si="4"/>
-        <v>21.619999</v>
-      </c>
-      <c r="E11" s="19">
-        <f t="shared" si="2"/>
-        <v>864.79996000000006</v>
-      </c>
-      <c r="F11" s="26">
-        <f t="shared" si="3"/>
-        <v>135.84246005803735</v>
+        <v>150.32524617338345</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2624,16 +2622,16 @@
         <v>0.17671458374999999</v>
       </c>
       <c r="D12" s="21">
+        <f t="shared" si="2"/>
+        <v>25.374146</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="3"/>
+        <v>902.19185777777784</v>
+      </c>
+      <c r="F12" s="23">
         <f t="shared" si="4"/>
-        <v>22.582768000000002</v>
-      </c>
-      <c r="E12" s="10">
-        <f t="shared" si="2"/>
-        <v>802.9428622222224</v>
-      </c>
-      <c r="F12" s="26">
-        <f t="shared" si="3"/>
-        <v>141.89171609304535</v>
+        <v>159.43046132942968</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -2676,16 +2674,16 @@
         <v>0.1963495375</v>
       </c>
       <c r="D13" s="21">
+        <f t="shared" si="2"/>
+        <v>26.104161000000001</v>
+      </c>
+      <c r="E13" s="19">
+        <f t="shared" si="3"/>
+        <v>835.33315200000004</v>
+      </c>
+      <c r="F13" s="23">
         <f t="shared" si="4"/>
-        <v>23.925006</v>
-      </c>
-      <c r="E13" s="19">
-        <f t="shared" si="2"/>
-        <v>765.60019199999999</v>
-      </c>
-      <c r="F13" s="26">
-        <f t="shared" si="3"/>
-        <v>150.32524617338345</v>
+        <v>164.01728085145038</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -2728,16 +2726,16 @@
         <v>0.21598449125000002</v>
       </c>
       <c r="D14" s="21">
+        <f t="shared" si="2"/>
+        <v>38.663786000000002</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="3"/>
+        <v>1124.7646836363635</v>
+      </c>
+      <c r="F14" s="23">
         <f t="shared" si="4"/>
-        <v>25.374146</v>
-      </c>
-      <c r="E14" s="10">
-        <f t="shared" si="2"/>
-        <v>738.15697454545455</v>
-      </c>
-      <c r="F14" s="26">
-        <f t="shared" si="3"/>
-        <v>159.43046132942968</v>
+        <v>242.93173211513579</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -2780,16 +2778,16 @@
         <v>0.23561944499999998</v>
       </c>
       <c r="D15" s="21">
+        <f t="shared" si="2"/>
+        <v>42.185623999999997</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="3"/>
+        <v>1124.9499733333332</v>
+      </c>
+      <c r="F15" s="23">
         <f t="shared" si="4"/>
-        <v>26.104161000000001</v>
-      </c>
-      <c r="E15" s="10">
-        <f t="shared" si="2"/>
-        <v>696.11096000000009</v>
-      </c>
-      <c r="F15" s="26">
-        <f t="shared" si="3"/>
-        <v>164.01728085145038</v>
+        <v>265.06009289100251</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -2832,16 +2830,16 @@
         <v>0.25525439875</v>
       </c>
       <c r="D16" s="21">
+        <f t="shared" si="2"/>
+        <v>46.907986000000001</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="3"/>
+        <v>1154.6581169230769</v>
+      </c>
+      <c r="F16" s="23">
         <f t="shared" si="4"/>
-        <v>38.663786000000002</v>
-      </c>
-      <c r="E16" s="10">
-        <f t="shared" si="2"/>
-        <v>951.72396307692316</v>
-      </c>
-      <c r="F16" s="26">
-        <f t="shared" si="3"/>
-        <v>242.93173211513579</v>
+        <v>294.73156842458576</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -2884,16 +2882,16 @@
         <v>0.27488935250000002</v>
       </c>
       <c r="D17" s="21">
+        <f t="shared" si="2"/>
+        <v>52.444453000000003</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="3"/>
+        <v>1198.7303542857144</v>
+      </c>
+      <c r="F17" s="23">
         <f t="shared" si="4"/>
-        <v>42.185623999999997</v>
-      </c>
-      <c r="E17" s="10">
-        <f t="shared" si="2"/>
-        <v>964.24283428571414</v>
-      </c>
-      <c r="F17" s="26">
-        <f t="shared" si="3"/>
-        <v>265.06009289100251</v>
+        <v>329.51821653267041</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -2936,16 +2934,16 @@
         <v>0.29452430625000003</v>
       </c>
       <c r="D18" s="21">
+        <f t="shared" si="2"/>
+        <v>58.627513</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="3"/>
+        <v>1250.7202773333333</v>
+      </c>
+      <c r="F18" s="23">
         <f t="shared" si="4"/>
-        <v>46.907986000000001</v>
-      </c>
-      <c r="E18" s="10">
-        <f t="shared" si="2"/>
-        <v>1000.7037013333332</v>
-      </c>
-      <c r="F18" s="26">
-        <f t="shared" si="3"/>
-        <v>294.73156842458576</v>
+        <v>368.36752827808021</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -2988,16 +2986,16 @@
         <v>0.31415926</v>
       </c>
       <c r="D19" s="21">
+        <f t="shared" si="2"/>
+        <v>65.365920000000003</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="3"/>
+        <v>1307.3184000000001</v>
+      </c>
+      <c r="F19" s="23">
         <f t="shared" si="4"/>
-        <v>52.444453000000003</v>
-      </c>
-      <c r="E19" s="10">
-        <f t="shared" si="2"/>
-        <v>1048.8890600000002</v>
-      </c>
-      <c r="F19" s="26">
-        <f t="shared" si="3"/>
-        <v>329.51821653267041</v>
+        <v>410.70618813427626</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -3040,16 +3038,16 @@
         <v>0.33379421375000001</v>
       </c>
       <c r="D20" s="21">
+        <f t="shared" si="2"/>
+        <v>72.598113999999995</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" si="3"/>
+        <v>1366.5527341176469</v>
+      </c>
+      <c r="F20" s="23">
         <f t="shared" si="4"/>
-        <v>58.627513</v>
-      </c>
-      <c r="E20" s="19">
-        <f t="shared" si="2"/>
-        <v>1103.5767152941178</v>
-      </c>
-      <c r="F20" s="26">
-        <f t="shared" si="3"/>
-        <v>368.36752827808021</v>
+        <v>456.14740321374859</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -3092,16 +3090,16 @@
         <v>0.35342916749999997</v>
       </c>
       <c r="D21" s="21">
+        <f t="shared" si="2"/>
+        <v>80.270891000000006</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="3"/>
+        <v>1427.0380622222224</v>
+      </c>
+      <c r="F21" s="23">
         <f t="shared" si="4"/>
-        <v>65.365920000000003</v>
-      </c>
-      <c r="E21" s="10">
-        <f t="shared" si="2"/>
-        <v>1162.0608000000002</v>
-      </c>
-      <c r="F21" s="26">
-        <f t="shared" si="3"/>
-        <v>410.70618813427626</v>
+        <v>504.35688292541414</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -3144,16 +3142,16 @@
         <v>0.37306412125000005</v>
       </c>
       <c r="D22" s="21">
+        <f t="shared" si="2"/>
+        <v>88.296522999999993</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="3"/>
+        <v>1487.0993347368419</v>
+      </c>
+      <c r="F22" s="23">
         <f t="shared" si="4"/>
-        <v>72.598113999999995</v>
-      </c>
-      <c r="E22" s="10">
-        <f t="shared" si="2"/>
-        <v>1222.7050778947366</v>
-      </c>
-      <c r="F22" s="26">
-        <f t="shared" si="3"/>
-        <v>456.14740321374859</v>
+        <v>554.78341598864438</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -3196,16 +3194,16 @@
         <v>0.39269907500000001</v>
       </c>
       <c r="D23" s="21">
+        <f t="shared" si="2"/>
+        <v>99.046975000000003</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="3"/>
+        <v>1584.7516000000001</v>
+      </c>
+      <c r="F23" s="23">
         <f t="shared" si="4"/>
-        <v>80.270891000000006</v>
-      </c>
-      <c r="E23" s="10">
-        <f t="shared" si="2"/>
-        <v>1284.3342560000001</v>
-      </c>
-      <c r="F23" s="26">
-        <f t="shared" si="3"/>
-        <v>504.35688292541414</v>
+        <v>622.33049804058385</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -3248,16 +3246,16 @@
         <v>0.41233402875000003</v>
       </c>
       <c r="D24" s="21">
+        <f t="shared" si="2"/>
+        <v>106.19070000000001</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="3"/>
+        <v>1618.1440000000002</v>
+      </c>
+      <c r="F24" s="23">
         <f t="shared" si="4"/>
-        <v>88.296522999999993</v>
-      </c>
-      <c r="E24" s="10">
-        <f t="shared" si="2"/>
-        <v>1345.4708266666667</v>
-      </c>
-      <c r="F24" s="26">
-        <f t="shared" si="3"/>
-        <v>554.78341598864438</v>
+        <v>667.21584599911534</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -3300,16 +3298,16 @@
         <v>0.43196898250000004</v>
       </c>
       <c r="D25" s="21">
+        <f t="shared" si="2"/>
+        <v>115.34310000000001</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="3"/>
+        <v>1677.7178181818183</v>
+      </c>
+      <c r="F25" s="23">
         <f t="shared" si="4"/>
-        <v>99.046975000000003</v>
-      </c>
-      <c r="E25" s="10">
-        <f t="shared" si="2"/>
-        <v>1440.6832727272727</v>
-      </c>
-      <c r="F25" s="26">
-        <f t="shared" si="3"/>
-        <v>622.33049804058385</v>
+        <v>724.72207120454573</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -3352,16 +3350,16 @@
         <v>0.45160393625</v>
       </c>
       <c r="D26" s="21">
+        <f t="shared" si="2"/>
+        <v>124.90152</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="3"/>
+        <v>1737.7602782608697</v>
+      </c>
+      <c r="F26" s="23">
         <f t="shared" si="4"/>
-        <v>106.19070000000001</v>
-      </c>
-      <c r="E26" s="10">
-        <f t="shared" si="2"/>
-        <v>1477.4358260869567</v>
-      </c>
-      <c r="F26" s="26">
-        <f t="shared" si="3"/>
-        <v>667.21584599911534</v>
+        <v>784.77939530839728</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -3404,16 +3402,16 @@
         <v>0.47123888999999997</v>
       </c>
       <c r="D27" s="21">
+        <f t="shared" si="2"/>
+        <v>134.79088999999999</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="3"/>
+        <v>1797.2118666666665</v>
+      </c>
+      <c r="F27" s="23">
         <f t="shared" si="4"/>
-        <v>115.34310000000001</v>
-      </c>
-      <c r="E27" s="10">
-        <f t="shared" si="2"/>
-        <v>1537.9080000000004</v>
-      </c>
-      <c r="F27" s="26">
-        <f t="shared" si="3"/>
-        <v>724.72207120454573</v>
+        <v>846.91613958965979</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -3456,16 +3454,16 @@
         <v>0.49087384374999998</v>
       </c>
       <c r="D28" s="21">
+        <f t="shared" si="2"/>
+        <v>144.97841</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="3"/>
+        <v>1855.7236479999999</v>
+      </c>
+      <c r="F28" s="23">
         <f t="shared" si="4"/>
-        <v>124.90152</v>
-      </c>
-      <c r="E28" s="10">
-        <f t="shared" si="2"/>
-        <v>1598.7394560000002</v>
-      </c>
-      <c r="F28" s="26">
-        <f t="shared" si="3"/>
-        <v>784.77939530839728</v>
+        <v>910.92621557025802</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -3508,16 +3506,16 @@
         <v>0.5105087975</v>
       </c>
       <c r="D29" s="21">
+        <f t="shared" si="2"/>
+        <v>155.43450999999999</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" si="3"/>
+        <v>1913.040123076923</v>
+      </c>
+      <c r="F29" s="23">
         <f t="shared" si="4"/>
-        <v>134.79088999999999</v>
-      </c>
-      <c r="E29" s="10">
-        <f t="shared" si="2"/>
-        <v>1658.9647999999997</v>
-      </c>
-      <c r="F29" s="26">
-        <f t="shared" si="3"/>
-        <v>846.91613958965979</v>
+        <v>976.62382946065838</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -3560,16 +3558,16 @@
         <v>0.53014375125000002</v>
       </c>
       <c r="D30" s="21">
+        <f t="shared" si="2"/>
+        <v>166.11924999999999</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="3"/>
+        <v>1968.8207407407408</v>
+      </c>
+      <c r="F30" s="23">
         <f t="shared" si="4"/>
-        <v>144.97841</v>
-      </c>
-      <c r="E30" s="10">
-        <f t="shared" si="2"/>
-        <v>1718.2626370370369</v>
-      </c>
-      <c r="F30" s="26">
-        <f t="shared" si="3"/>
-        <v>910.92621557025802</v>
+        <v>1043.7580308396925</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -3612,16 +3610,16 @@
         <v>0.54977870500000003</v>
       </c>
       <c r="D31" s="21">
+        <f t="shared" si="2"/>
+        <v>176.94967</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="3"/>
+        <v>2022.2819428571427</v>
+      </c>
+      <c r="F31" s="23">
         <f t="shared" si="4"/>
-        <v>155.43450999999999</v>
-      </c>
-      <c r="E31" s="10">
-        <f t="shared" si="2"/>
-        <v>1776.3943999999997</v>
-      </c>
-      <c r="F31" s="26">
-        <f t="shared" si="3"/>
-        <v>976.62382946065838</v>
+        <v>1111.8075666542763</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -3664,16 +3662,16 @@
         <v>0.56941365874999994</v>
       </c>
       <c r="D32" s="21">
+        <f t="shared" si="2"/>
+        <v>187.60668000000001</v>
+      </c>
+      <c r="E32" s="19">
+        <f t="shared" si="3"/>
+        <v>2070.1426758620696</v>
+      </c>
+      <c r="F32" s="23">
         <f t="shared" si="4"/>
-        <v>166.11924999999999</v>
-      </c>
-      <c r="E32" s="19">
-        <f t="shared" si="2"/>
-        <v>1833.0400000000002</v>
-      </c>
-      <c r="F32" s="26">
-        <f t="shared" si="3"/>
-        <v>1043.7580308396925</v>
+        <v>1178.7675353047423</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -3716,16 +3714,16 @@
         <v>0.58904861250000007</v>
       </c>
       <c r="D33" s="21">
+        <f t="shared" si="2"/>
+        <v>206.29392999999999</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="3"/>
+        <v>2200.4685866666664</v>
+      </c>
+      <c r="F33" s="23">
         <f t="shared" si="4"/>
-        <v>176.94967</v>
-      </c>
-      <c r="E33" s="10">
-        <f t="shared" si="2"/>
-        <v>1887.4631466666663</v>
-      </c>
-      <c r="F33" s="26">
-        <f t="shared" si="3"/>
-        <v>1111.8075666542763</v>
+        <v>1296.182989936334</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -3768,16 +3766,16 @@
         <v>0.60868356625000009</v>
       </c>
       <c r="D34" s="21">
+        <f t="shared" si="2"/>
+        <v>213.61906999999999</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="3"/>
+        <v>2205.1000774193544</v>
+      </c>
+      <c r="F34" s="23">
         <f t="shared" si="4"/>
-        <v>187.60668000000001</v>
-      </c>
-      <c r="E34" s="10">
-        <f t="shared" si="2"/>
-        <v>1936.5850838709678</v>
-      </c>
-      <c r="F34" s="26">
-        <f t="shared" si="3"/>
-        <v>1178.7675353047423</v>
+        <v>1342.2082019573675</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -3820,16 +3818,16 @@
         <v>0.62831851999999999</v>
       </c>
       <c r="D35" s="21">
+        <f t="shared" si="2"/>
+        <v>224.92605</v>
+      </c>
+      <c r="E35" s="10">
+        <f t="shared" si="3"/>
+        <v>2249.2605000000003</v>
+      </c>
+      <c r="F35" s="23">
         <f t="shared" si="4"/>
-        <v>206.29392999999999</v>
-      </c>
-      <c r="E35" s="10">
-        <f t="shared" si="2"/>
-        <v>2062.9393</v>
-      </c>
-      <c r="F35" s="26">
-        <f t="shared" si="3"/>
-        <v>1296.182989936334</v>
+        <v>1413.2520525619409</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -3872,16 +3870,16 @@
         <v>0.64795347375000001</v>
       </c>
       <c r="D36" s="21">
+        <f t="shared" si="2"/>
+        <v>236.83924999999999</v>
+      </c>
+      <c r="E36" s="10">
+        <f t="shared" si="3"/>
+        <v>2296.6230303030302</v>
+      </c>
+      <c r="F36" s="23">
         <f t="shared" si="4"/>
-        <v>213.61906999999999</v>
-      </c>
-      <c r="E36" s="10">
-        <f t="shared" si="2"/>
-        <v>2071.4576484848485</v>
-      </c>
-      <c r="F36" s="26">
-        <f t="shared" si="3"/>
-        <v>1342.2082019573675</v>
+        <v>1488.1048957634328</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -3924,16 +3922,16 @@
         <v>0.66758842750000003</v>
       </c>
       <c r="D37" s="21">
+        <f t="shared" si="2"/>
+        <v>249.03820999999999</v>
+      </c>
+      <c r="E37" s="10">
+        <f t="shared" si="3"/>
+        <v>2343.8890352941175</v>
+      </c>
+      <c r="F37" s="23">
         <f t="shared" si="4"/>
-        <v>224.92605</v>
-      </c>
-      <c r="E37" s="10">
-        <f t="shared" si="2"/>
-        <v>2116.9510588235294</v>
-      </c>
-      <c r="F37" s="26">
-        <f t="shared" si="3"/>
-        <v>1413.2520525619409</v>
+        <v>1564.7532219983043</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -3976,16 +3974,16 @@
         <v>0.68722338125000004</v>
       </c>
       <c r="D38" s="21">
+        <f t="shared" si="2"/>
+        <v>261.43599</v>
+      </c>
+      <c r="E38" s="10">
+        <f t="shared" si="3"/>
+        <v>2390.2719085714284</v>
+      </c>
+      <c r="F38" s="23">
         <f t="shared" si="4"/>
-        <v>236.83924999999999</v>
-      </c>
-      <c r="E38" s="10">
-        <f t="shared" si="2"/>
-        <v>2165.3874285714282</v>
-      </c>
-      <c r="F38" s="26">
-        <f t="shared" si="3"/>
-        <v>1488.1048957634328</v>
+        <v>1642.6507711359493</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -4028,16 +4026,16 @@
         <v>0.70685833499999995</v>
       </c>
       <c r="D39" s="21">
+        <f t="shared" si="2"/>
+        <v>273.98219</v>
+      </c>
+      <c r="E39" s="10">
+        <f t="shared" si="3"/>
+        <v>2435.3972444444448</v>
+      </c>
+      <c r="F39" s="23">
         <f t="shared" si="4"/>
-        <v>249.03820999999999</v>
-      </c>
-      <c r="E39" s="10">
-        <f t="shared" si="2"/>
-        <v>2213.6729777777778</v>
-      </c>
-      <c r="F39" s="26">
-        <f t="shared" si="3"/>
-        <v>1564.7532219983043</v>
+        <v>1721.4808706368858</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -4080,16 +4078,16 @@
         <v>0.72649328874999997</v>
       </c>
       <c r="D40" s="21">
+        <f t="shared" si="2"/>
+        <v>286.61851000000001</v>
+      </c>
+      <c r="E40" s="10">
+        <f t="shared" si="3"/>
+        <v>2478.8627891891892</v>
+      </c>
+      <c r="F40" s="23">
         <f t="shared" si="4"/>
-        <v>261.43599</v>
-      </c>
-      <c r="E40" s="10">
-        <f t="shared" si="2"/>
-        <v>2261.0680216216215</v>
-      </c>
-      <c r="F40" s="26">
-        <f t="shared" si="3"/>
-        <v>1642.6507711359493</v>
+        <v>1800.8772107977054</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -4132,16 +4130,16 @@
         <v>0.74612824250000009</v>
       </c>
       <c r="D41" s="21">
+        <f t="shared" si="2"/>
+        <v>299.22075999999998</v>
+      </c>
+      <c r="E41" s="19">
+        <f t="shared" si="3"/>
+        <v>2519.7537684210524</v>
+      </c>
+      <c r="F41" s="23">
         <f t="shared" si="4"/>
-        <v>273.98219</v>
-      </c>
-      <c r="E41" s="19">
-        <f t="shared" si="2"/>
-        <v>2307.218442105263</v>
-      </c>
-      <c r="F41" s="26">
-        <f t="shared" si="3"/>
-        <v>1721.4808706368858</v>
+        <v>1880.0594828351091</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -4184,16 +4182,16 @@
         <v>0.76576319625000011</v>
       </c>
       <c r="D42" s="21">
+        <f t="shared" si="2"/>
+        <v>311.30452000000002</v>
+      </c>
+      <c r="E42" s="10">
+        <f t="shared" si="3"/>
+        <v>2554.2934974358973</v>
+      </c>
+      <c r="F42" s="23">
         <f t="shared" si="4"/>
-        <v>286.61851000000001</v>
-      </c>
-      <c r="E42" s="10">
-        <f t="shared" si="2"/>
-        <v>2351.7416205128202</v>
-      </c>
-      <c r="F42" s="26">
-        <f t="shared" si="3"/>
-        <v>1800.8772107977054</v>
+        <v>1955.9839861225937</v>
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -4236,16 +4234,16 @@
         <v>0.78539815000000002</v>
       </c>
       <c r="D43" s="21">
+        <f t="shared" si="2"/>
+        <v>334.74155000000002</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="3"/>
+        <v>2677.9324000000006</v>
+      </c>
+      <c r="F43" s="23">
         <f t="shared" si="4"/>
-        <v>299.22075999999998</v>
-      </c>
-      <c r="E43" s="10">
-        <f t="shared" si="2"/>
-        <v>2393.7660799999999</v>
-      </c>
-      <c r="F43" s="26">
-        <f t="shared" si="3"/>
-        <v>1880.0594828351091</v>
+        <v>2103.2431886625209</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -4288,16 +4286,16 @@
         <v>0.80503310375000003</v>
       </c>
       <c r="D44" s="21">
+        <f t="shared" si="2"/>
+        <v>342.33744999999999</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="3"/>
+        <v>2671.9020487804878</v>
+      </c>
+      <c r="F44" s="23">
         <f t="shared" si="4"/>
-        <v>311.30452000000002</v>
-      </c>
-      <c r="E44" s="10">
-        <f t="shared" si="2"/>
-        <v>2429.6938146341463</v>
-      </c>
-      <c r="F44" s="26">
-        <f t="shared" si="3"/>
-        <v>1955.9839861225937</v>
+        <v>2150.9696359373261</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -4340,16 +4338,16 @@
         <v>0.82466805750000005</v>
       </c>
       <c r="D45" s="21">
+        <f t="shared" si="2"/>
+        <v>354.7715</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="3"/>
+        <v>2703.0209523809526</v>
+      </c>
+      <c r="F45" s="23">
         <f t="shared" si="4"/>
-        <v>334.74155000000002</v>
-      </c>
-      <c r="E45" s="10">
-        <f t="shared" si="2"/>
-        <v>2550.41180952381</v>
-      </c>
-      <c r="F45" s="26">
-        <f t="shared" si="3"/>
-        <v>2103.2431886625209</v>
+        <v>2229.0950762060625</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -4392,16 +4390,16 @@
         <v>0.84430301125000007</v>
       </c>
       <c r="D46" s="21">
+        <f t="shared" si="2"/>
+        <v>367.95744999999999</v>
+      </c>
+      <c r="E46" s="10">
+        <f t="shared" si="3"/>
+        <v>2738.2879999999996</v>
+      </c>
+      <c r="F46" s="23">
         <f t="shared" si="4"/>
-        <v>342.33744999999999</v>
-      </c>
-      <c r="E46" s="10">
-        <f t="shared" si="2"/>
-        <v>2547.6275348837207</v>
-      </c>
-      <c r="F46" s="26">
-        <f t="shared" si="3"/>
-        <v>2150.9696359373261</v>
+        <v>2311.9448435072673</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -4444,16 +4442,16 @@
         <v>0.86393796500000009</v>
       </c>
       <c r="D47" s="21">
+        <f t="shared" si="2"/>
+        <v>381.41021999999998</v>
+      </c>
+      <c r="E47" s="10">
+        <f t="shared" si="3"/>
+        <v>2773.8925090909083</v>
+      </c>
+      <c r="F47" s="23">
         <f t="shared" si="4"/>
-        <v>354.7715</v>
-      </c>
-      <c r="E47" s="10">
-        <f t="shared" si="2"/>
-        <v>2580.1563636363635</v>
-      </c>
-      <c r="F47" s="26">
-        <f t="shared" si="3"/>
-        <v>2229.0950762060625</v>
+        <v>2396.4710903121336</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -4496,16 +4494,16 @@
         <v>0.8835729187500001</v>
       </c>
       <c r="D48" s="21">
+        <f t="shared" si="2"/>
+        <v>395.00335999999999</v>
+      </c>
+      <c r="E48" s="10">
+        <f t="shared" si="3"/>
+        <v>2808.9127822222222</v>
+      </c>
+      <c r="F48" s="23">
         <f t="shared" si="4"/>
-        <v>367.95744999999999</v>
-      </c>
-      <c r="E48" s="10">
-        <f t="shared" si="2"/>
-        <v>2616.5863111111107</v>
-      </c>
-      <c r="F48" s="26">
-        <f t="shared" si="3"/>
-        <v>2311.9448435072673</v>
+        <v>2481.8793078385688</v>
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
@@ -4548,16 +4546,16 @@
         <v>0.90320787250000001</v>
       </c>
       <c r="D49" s="21">
+        <f t="shared" si="2"/>
+        <v>392.51524999999998</v>
+      </c>
+      <c r="E49" s="10">
+        <f t="shared" si="3"/>
+        <v>2730.5408695652172</v>
+      </c>
+      <c r="F49" s="23">
         <f t="shared" si="4"/>
-        <v>381.41021999999998</v>
-      </c>
-      <c r="E49" s="10">
-        <f t="shared" si="2"/>
-        <v>2653.2884869565214</v>
-      </c>
-      <c r="F49" s="26">
-        <f t="shared" si="3"/>
-        <v>2396.4710903121336</v>
+        <v>2466.2460516439219</v>
       </c>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -4600,16 +4598,16 @@
         <v>0.92284282625000003</v>
       </c>
       <c r="D50" s="21">
+        <f t="shared" si="2"/>
+        <v>405.74435</v>
+      </c>
+      <c r="E50" s="10">
+        <f t="shared" si="3"/>
+        <v>2762.5147234042552</v>
+      </c>
+      <c r="F50" s="23">
         <f t="shared" si="4"/>
-        <v>395.00335999999999</v>
-      </c>
-      <c r="E50" s="10">
-        <f t="shared" si="2"/>
-        <v>2689.3845787234045</v>
-      </c>
-      <c r="F50" s="26">
-        <f t="shared" si="3"/>
-        <v>2481.8793078385688</v>
+        <v>2549.3669383911315</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -4652,16 +4650,16 @@
         <v>0.94247777999999993</v>
       </c>
       <c r="D51" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="23">
         <f t="shared" si="4"/>
-        <v>392.51524999999998</v>
-      </c>
-      <c r="E51" s="10">
-        <f t="shared" si="2"/>
-        <v>2616.7683333333334</v>
-      </c>
-      <c r="F51" s="26">
-        <f t="shared" si="3"/>
-        <v>2466.2460516439219</v>
+        <v>0</v>
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
@@ -4704,16 +4702,16 @@
         <v>0.96211273374999995</v>
       </c>
       <c r="D52" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="23">
         <f t="shared" si="4"/>
-        <v>405.74435</v>
-      </c>
-      <c r="E52" s="10">
-        <f t="shared" si="2"/>
-        <v>2649.7590204081635</v>
-      </c>
-      <c r="F52" s="26">
-        <f t="shared" si="3"/>
-        <v>2549.3669383911315</v>
+        <v>0</v>
       </c>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -4756,15 +4754,15 @@
         <v>0.98174768749999997</v>
       </c>
       <c r="D53" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F53" s="26">
+      <c r="E53" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G53" s="6"/>
@@ -4808,15 +4806,15 @@
         <v>1.00138264125</v>
       </c>
       <c r="D54" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F54" s="26">
+      <c r="E54" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G54" s="6"/>
@@ -4844,15 +4842,15 @@
         <v>1.021017595</v>
       </c>
       <c r="D55" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F55" s="26">
+      <c r="E55" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G55" s="6"/>
@@ -4880,15 +4878,15 @@
         <v>1.04065254875</v>
       </c>
       <c r="D56" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E56" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F56" s="26">
+      <c r="E56" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G56" s="6"/>
@@ -4916,15 +4914,15 @@
         <v>1.0602875025</v>
       </c>
       <c r="D57" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E57" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F57" s="26">
+      <c r="E57" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G57" s="6"/>
@@ -4952,15 +4950,15 @@
         <v>1.0799224562500001</v>
       </c>
       <c r="D58" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E58" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F58" s="26">
+      <c r="E58" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G58" s="6"/>
@@ -4980,7 +4978,7 @@
       <c r="B59" s="6"/>
       <c r="C59" s="5"/>
       <c r="E59" s="5"/>
-      <c r="F59" s="27"/>
+      <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -4999,7 +4997,7 @@
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
-      <c r="F60" s="27"/>
+      <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
@@ -5018,7 +5016,7 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
-      <c r="F61" s="27"/>
+      <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -5037,7 +5035,7 @@
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-      <c r="F62" s="27"/>
+      <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -5056,7 +5054,7 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-      <c r="F63" s="27"/>
+      <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
@@ -5075,7 +5073,7 @@
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
-      <c r="F64" s="27"/>
+      <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
@@ -5094,7 +5092,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
-      <c r="F65" s="27"/>
+      <c r="F65" s="6"/>
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
@@ -5113,7 +5111,7 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
-      <c r="F66" s="27"/>
+      <c r="F66" s="6"/>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
@@ -5132,7 +5130,7 @@
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
-      <c r="F67" s="27"/>
+      <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
@@ -5151,7 +5149,7 @@
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
-      <c r="F68" s="27"/>
+      <c r="F68" s="6"/>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
@@ -5170,7 +5168,7 @@
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
-      <c r="F69" s="27"/>
+      <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
@@ -5189,7 +5187,7 @@
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
-      <c r="F70" s="27"/>
+      <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
@@ -5208,7 +5206,7 @@
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
-      <c r="F71" s="27"/>
+      <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
@@ -5227,7 +5225,7 @@
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
-      <c r="F72" s="27"/>
+      <c r="F72" s="6"/>
       <c r="G72" s="6"/>
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
@@ -5246,7 +5244,7 @@
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
-      <c r="F73" s="27"/>
+      <c r="F73" s="6"/>
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>

</xml_diff>

<commit_message>
some more files for ML Part B
</commit_message>
<xml_diff>
--- a/3_ML/Part B - Matlab Model/wavenumber-frequency curve.xlsx
+++ b/3_ML/Part B - Matlab Model/wavenumber-frequency curve.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{6A15CA82-5337-48B6-BCBF-DA78EBE36219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFD56D1E-9AD7-417D-B317-41794BB7EF32}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{6A15CA82-5337-48B6-BCBF-DA78EBE36219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5C4B3BA-9C19-47DB-B2D9-F9F86D983D42}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>order</t>
   </si>
@@ -261,9 +261,6 @@
     <t>https://support.microsoft.com/en-us/office/split-text-into-different-columns-with-the-convert-text-to-columns-wizard-30b14928-5550-41f5-97ca-7a3e9c363ed7</t>
   </si>
   <si>
-    <t>L=160, wavelength is 2/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">     SET   TIME/FREQ    LOAD STEP   SUBSTEP  CUMULATIVE</t>
   </si>
   <si>
@@ -390,10 +387,10 @@
     <t xml:space="preserve">      74  395.00336             1        74        74                  </t>
   </si>
   <si>
-    <t>HOW TO DETERMINE??</t>
-  </si>
-  <si>
     <t>omega</t>
+  </si>
+  <si>
+    <t>min value</t>
   </si>
 </sst>
 </file>
@@ -1110,6 +1107,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>wave number [m⁻¹]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1172,6 +1224,765 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>angular frequency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> [rad/s²]</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764915048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Dispersion curve</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>1.963495375E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9269907499999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8904861249999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8539814999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8174768750000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11780972249999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13744467625000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15707963</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17671458374999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1963495375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.21598449125000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.23561944499999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25525439875</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27488935250000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29452430625000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.31415926</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.33379421375000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.35342916749999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.37306412125000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.39269907500000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.41233402875000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.43196898250000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.45160393625</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.47123888999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.49087384374999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5105087975</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.53014375125000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.54977870500000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.56941365874999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.58904861250000007</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.60868356625000009</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.62831851999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.64795347375000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.66758842750000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.68722338125000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.70685833499999995</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.72649328874999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.74612824250000009</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.76576319625000011</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.78539815000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.80503310375000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.82466805750000005</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.84430301125000007</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.86393796500000009</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.8835729187500001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.90320787250000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.92284282625000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>6635.180800000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3323.7555200000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2217.9078399999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1666.3238400000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1347.262144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1153.0666133333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1032.3551085714287</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>957.00023999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>902.19185777777784</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>835.33315200000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1124.7646836363635</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1124.9499733333332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1154.6581169230769</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1198.7303542857144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1250.7202773333333</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1307.3184000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1366.5527341176469</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1427.0380622222224</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1487.0993347368419</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1584.7516000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1618.1440000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1677.7178181818183</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1737.7602782608697</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1797.2118666666665</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1855.7236479999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1913.040123076923</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1968.8207407407408</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2022.2819428571427</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2070.1426758620696</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2200.4685866666664</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2205.1000774193544</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2249.2605000000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2296.6230303030302</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2343.8890352941175</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2390.2719085714284</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2435.3972444444448</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2478.8627891891892</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2519.7537684210524</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2554.2934974358973</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2677.9324000000006</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2671.9020487804878</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2703.0209523809526</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2738.2879999999996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2773.8925090909083</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2808.9127822222222</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2730.5408695652172</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2762.5147234042552</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B4E9-401D-BBEB-9A1EE6356452}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="764915048"/>
+        <c:axId val="764915704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="764915048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>wave number [m⁻¹]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764915704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="764915704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>phase speed [m/s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1259,6 +2070,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1814,6 +2665,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1847,6 +3214,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5025458</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>13358</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1769FBDE-4329-4254-8FC8-C98B3B0D2898}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2120,8 +3525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2189,7 +3594,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
@@ -2319,7 +3724,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="6"/>
       <c r="M6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -2376,13 +3781,11 @@
       <c r="K7" s="15"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
-      <c r="P7" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="P7" s="6"/>
       <c r="R7">
         <v>2</v>
       </c>
@@ -2430,13 +3833,10 @@
       <c r="K8" s="15"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" t="s">
-        <v>70</v>
-      </c>
       <c r="R8">
         <v>3</v>
       </c>
@@ -2484,7 +3884,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -2536,7 +3936,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -2588,7 +3988,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -2640,7 +4040,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -2692,7 +4092,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -2744,7 +4144,7 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -2796,7 +4196,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
@@ -2900,7 +4300,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
@@ -2952,7 +4352,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -3004,7 +4404,7 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -3056,7 +4456,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -3108,7 +4508,7 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -3160,7 +4560,7 @@
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -3212,7 +4612,7 @@
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -3264,7 +4664,7 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -3316,7 +4716,7 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -3420,7 +4820,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
@@ -3472,7 +4872,7 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -3524,7 +4924,7 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -3576,7 +4976,7 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -3628,7 +5028,7 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
@@ -3680,7 +5080,7 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
@@ -3732,7 +5132,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
@@ -3784,7 +5184,7 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
@@ -3836,7 +5236,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
@@ -3940,7 +5340,7 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
@@ -3992,7 +5392,7 @@
       <c r="K38" s="7"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
@@ -4044,7 +5444,7 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
@@ -4096,7 +5496,7 @@
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
@@ -4148,7 +5548,7 @@
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
@@ -4200,7 +5600,7 @@
       <c r="K42" s="7"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
@@ -4252,7 +5652,7 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
@@ -4304,7 +5704,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
@@ -4356,7 +5756,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
@@ -4454,13 +5854,18 @@
         <v>2396.4710903121336</v>
       </c>
       <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
+      <c r="H47" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I47" s="23">
+        <f>MIN(E4:E50)</f>
+        <v>835.33315200000004</v>
+      </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
@@ -4512,7 +5917,7 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
@@ -4564,7 +5969,7 @@
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
@@ -4616,7 +6021,7 @@
       <c r="K50" s="7"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
@@ -4668,7 +6073,7 @@
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>

</xml_diff>